<commit_message>
updated xlsx and adding new rows to 'database'
</commit_message>
<xml_diff>
--- a/WestVSHubertBAZA.xlsx
+++ b/WestVSHubertBAZA.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\____DATA\_____PROJECTS\python\automate\MlodyWestVSHubert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3AC6B0-7C9B-4A34-A8F4-EB08717B33AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403B239D-9855-4FFC-B265-FA8C98F7F1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Liczby" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Rok</t>
   </si>
   <si>
     <t>Miesiąc</t>
+  </si>
+  <si>
+    <t>Dzien</t>
   </si>
   <si>
     <t>MłodyWest</t>
@@ -360,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,9 +388,52 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2138</v>
+      </c>
+      <c r="B2">
+        <v>2024</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>154720</v>
+      </c>
+      <c r="F2">
+        <v>148783</v>
+      </c>
+      <c r="G2">
+        <v>5937</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1276DAE4-9B14-4523-8DBB-EAC6532A8D24}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>